<commit_message>
Test cases another update
</commit_message>
<xml_diff>
--- a/FlightSearch.xlsx
+++ b/FlightSearch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BAA6F3-974D-4E43-AA11-1AD53EFA4395}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48E26EC-8F73-4432-8803-36BDD855A69B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="SEARCH_2_ReturnNoDepartureDate" sheetId="9" r:id="rId12"/>
     <sheet name="SEARCH_2_ReturnNoArrivalDate" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="145">
   <si>
     <t>PROJECT</t>
   </si>
@@ -412,16 +412,61 @@
     <t>Possible flights date from Wrocław to London on 9.11.2018 and possible flights from London to Wrocław on 11.11.2022</t>
   </si>
   <si>
-    <t>One way flight option marked. No return data field</t>
-  </si>
-  <si>
     <t>Wrocław and London found on airports list</t>
   </si>
   <si>
-    <t>Possible flight date from Wrocław to London are displayed</t>
+    <t>Returns exact time of flights on particular date</t>
   </si>
   <si>
-    <t>Returns exact time of flights on particular date</t>
+    <t>One way flight option marked. No return data field will be displayed</t>
+  </si>
+  <si>
+    <t>One way flight option marked. No return data field displayed</t>
+  </si>
+  <si>
+    <t>Wrocław and London will be found on airports list</t>
+  </si>
+  <si>
+    <t>Possible flight date from Wrocław to London will be displayed</t>
+  </si>
+  <si>
+    <t>Possible flight date from Wrocław to London is displayed</t>
+  </si>
+  <si>
+    <t>Will return exact time of flights on praticualr date</t>
+  </si>
+  <si>
+    <t>London will be found on airports list</t>
+  </si>
+  <si>
+    <t>London found on airports list</t>
+  </si>
+  <si>
+    <t>It is possible to provide date</t>
+  </si>
+  <si>
+    <t>There should be information that no departure city has been selected(NoError.png) but only button search is disabeld</t>
+  </si>
+  <si>
+    <t>2.  Provide Wrocław as departure</t>
+  </si>
+  <si>
+    <t>Wrocław will be found on airports list</t>
+  </si>
+  <si>
+    <t>Date field will be disabled because no destination airport has been selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select date field should be disabled, but it possible to provide date </t>
+  </si>
+  <si>
+    <t>Date slection field will be disabled because no departure airport has been selected</t>
+  </si>
+  <si>
+    <t>No return data field will be displayed</t>
+  </si>
+  <si>
+    <t>No return data field displayed</t>
   </si>
 </sst>
 </file>
@@ -693,7 +738,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Normalny 2" xfId="1" xr:uid="{197B7AA7-319A-4CB2-9511-8E2592BCCB12}"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="95">
     <dxf>
@@ -1417,7 +1462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -1452,7 +1497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -18293,7 +18338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65647DFC-4D98-4C65-BD12-03FE5E4F7818}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -18548,7 +18593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE7D7A9-6F73-4F6E-A6A0-310A2A52BF90}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18803,7 +18848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45DD5B-4563-4B70-B85B-34E6C3018917}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -19058,7 +19103,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09D37E1-3F49-47A0-BBBC-FB16DF367D18}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -19312,7 +19357,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B0E0D8-E5B8-4075-B3E7-32DBE68D9088}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19584,7 +19629,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE122FC-6A4F-472D-AFB4-3E463A66C1BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -19859,7 +19904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E88C7D-4FC7-4F65-839B-E8F149336215}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20041,11 +20086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDAE7B8-F38F-4799-8D14-50737728AAB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20158,7 +20203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -20178,52 +20223,97 @@
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>72</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>74</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>43</v>
@@ -20262,11 +20352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB6FF35F-96E3-496A-B7B4-F19414F8B417}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20379,7 +20469,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>52</v>
       </c>
@@ -20399,53 +20489,94 @@
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>57</v>
+        <v>144</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>75</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>58</v>
+        <v>134</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>74</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
@@ -20459,7 +20590,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -20495,11 +20626,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9741D50-4AEE-45D3-BFC6-BF01A15F6C84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20612,7 +20743,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>63</v>
       </c>
@@ -20628,57 +20759,98 @@
       <c r="E9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="10" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F10" s="6" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>74</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
@@ -20692,7 +20864,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -20728,7 +20900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1201DBF-776F-4E80-B326-18F6F5DF3A00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20969,7 +21141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770724BE-A242-4B78-9330-98FF62807E0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">

</xml_diff>